<commit_message>
Small format Tier description format change
</commit_message>
<xml_diff>
--- a/Tier System/stable version/v02-01/NBO-Microscopy Metadata Tier System_v02-01.xlsx
+++ b/Tier System/stable version/v02-01/NBO-Microscopy Metadata Tier System_v02-01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strambc/Documents/GitHub/NBOMicroscopyMetadataSpecs/Tier System/stable version/v02-00/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strambc/Documents/GitHub/NBOMicroscopyMetadataSpecs/Tier System/stable version/v02-01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E27409-C340-CE4E-A929-8EA3353F2AFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AFDAA2-64BC-144F-83C0-BA0A4E7FA161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28320" windowHeight="16740" tabRatio="914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Tier system_v02-00 MINIMAL" sheetId="14" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tier system_v02-00'!$A$1:$L$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tier system_v02-00'!$A$1:$L$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Tier system_v02-00 MINIMAL'!$A$2:$H$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Tier system_v02-00 SUMMARY'!$A$1:$J$5</definedName>
   </definedNames>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -191,13 +191,37 @@
   </si>
   <si>
     <t>Identification and localization of diffraction-limited particles, super-resolution microscopy, tracking of intracellular dynamics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplemental Table I: Extended view of the Tiers for the reporting of Light Microscopy Metadata as proposed by the Imaging Standards Working Group of the 4D Nucleome initiative and by the Quality Control and Data Management Working Group of Bioimaging North America. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Legend: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Each tier accommodates increasingly complex images, experiments, instrumentation, and analytical needs and therefore requires progressively more metadata. This tiered system is not intended to meet the needs of all imaging communities.  Rather it is proposed as a framework that might need to be adapted and modified depending on the needs of individual data collection consortia, disciplines, or institutions.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,6 +370,19 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -374,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -456,7 +493,7 @@
       </left>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -466,30 +503,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -644,6 +657,52 @@
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -684,7 +743,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -735,7 +794,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,13 +812,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -768,67 +827,58 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -837,7 +887,7 @@
     <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -858,31 +908,19 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -891,35 +929,62 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -1308,10 +1373,10 @@
     <tabColor theme="8" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="45" zoomScaleNormal="53" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="44" zoomScaleNormal="53" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection sqref="A1:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -1329,57 +1394,57 @@
     <col min="13" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+    <row r="1" spans="1:13" ht="127" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
     </row>
     <row r="2" spans="1:13" s="23" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="62" t="s">
+      <c r="H2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="62" t="s">
+      <c r="I2" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="62" t="s">
+      <c r="J2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="62" t="s">
+      <c r="K2" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="62" t="s">
+      <c r="L2" s="59" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="22"/>
@@ -1394,35 +1459,35 @@
       <c r="C3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="72" t="s">
+      <c r="K3" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="73"/>
+      <c r="L3" s="64"/>
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" s="10" customFormat="1" ht="406" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="61" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="29">
@@ -1431,72 +1496,91 @@
       <c r="C4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="K4" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="75"/>
+      <c r="L4" s="66"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" s="11" customFormat="1" ht="343" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
-      <c r="B5" s="17">
+      <c r="A5" s="61"/>
+      <c r="B5" s="74">
         <v>3</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="70"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="47" t="s">
+      <c r="H5" s="77"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="71" t="s">
+      <c r="K5" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="76"/>
+      <c r="L5" s="80"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="15"/>
-      <c r="I6" s="16"/>
+    <row r="6" spans="1:13" s="73" customFormat="1" ht="100" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C10" s="70"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C11" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="K3:L3"/>
@@ -1536,48 +1620,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:11" s="23" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="J2" s="55" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="22"/>
@@ -1598,7 +1682,7 @@
       <c r="E3" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="45" t="s">
         <v>43</v>
       </c>
       <c r="G3" s="36" t="s">
@@ -1616,7 +1700,7 @@
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" ht="359" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="61" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="29">
@@ -1649,7 +1733,7 @@
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" s="11" customFormat="1" ht="252" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -1665,11 +1749,11 @@
       <c r="F5" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="78"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="68"/>
       <c r="J5" s="20" t="s">
         <v>29</v>
       </c>
@@ -1718,28 +1802,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" s="23" customFormat="1" ht="107" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="55" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1753,24 +1837,24 @@
       <c r="C3" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="46" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="10" customFormat="1" ht="370" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="61" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="29">
@@ -1779,43 +1863,43 @@
       <c r="C4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="47" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1" ht="158" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="51" t="s">
         <v>29</v>
       </c>
       <c r="I5"/>

</xml_diff>